<commit_message>
added SS script with Kremp's update_prob script
</commit_message>
<xml_diff>
--- a/various_correlations_output.xlsx
+++ b/various_correlations_output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnrandolph/Desktop/Github/voting-power/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7951BD8-FB8B-FA4E-ADE5-F1D4D3EE1623}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B979AA6-3C22-3741-AB72-9B29DC7A30D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17800" windowHeight="22400" xr2:uid="{1A8CDEDC-9550-8544-A06A-66A54DD639E8}"/>
   </bookViews>
@@ -642,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3C4DDF8-C308-E94C-8C3B-BAAF738F897C}">
   <dimension ref="A1:AE55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V8" workbookViewId="0">
-      <selection activeCell="AC56" sqref="AC56"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AF13" sqref="AF13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>